<commit_message>
updated test query and resuls files
</commit_message>
<xml_diff>
--- a/new-table-builders/tests/test-2-return.xlsx
+++ b/new-table-builders/tests/test-2-return.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="38480" yWindow="3360" windowWidth="25360" windowHeight="17300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="display" sheetId="2" r:id="rId1"/>
-    <sheet name="export" sheetId="1" r:id="rId2"/>
+    <sheet name="display" sheetId="4" r:id="rId1"/>
+    <sheet name="export" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="58">
   <si>
     <t>targets count</t>
   </si>
@@ -110,16 +110,116 @@
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t>WP2309</t>
+  </si>
+  <si>
+    <t>WikiPathways_20170210</t>
+  </si>
+  <si>
+    <t>Mus musculus</t>
+  </si>
+  <si>
+    <t>WP523</t>
+  </si>
+  <si>
+    <t>WP2573</t>
+  </si>
+  <si>
+    <t>WP2310</t>
+  </si>
+  <si>
+    <t>WP2902</t>
+  </si>
+  <si>
+    <t>p53 signaling</t>
+  </si>
+  <si>
+    <t>WP385</t>
+  </si>
+  <si>
+    <t>WP2087</t>
+  </si>
+  <si>
+    <t>miRNA regulation of DNA Damage Response</t>
+  </si>
+  <si>
+    <t>WP2910</t>
+  </si>
+  <si>
+    <t>WP6</t>
+  </si>
+  <si>
+    <t>WP373</t>
+  </si>
+  <si>
+    <t>WP413</t>
+  </si>
+  <si>
+    <t>G1 to S cell cycle control</t>
+  </si>
+  <si>
+    <t>WP85</t>
+  </si>
+  <si>
+    <t>WP572</t>
+  </si>
+  <si>
+    <t>WP265</t>
+  </si>
+  <si>
+    <t>http://www.wikipathways.org/instance/WP2087_r86151</t>
+  </si>
+  <si>
+    <t>http://www.wikipathways.org/instance/WP2902_r88290</t>
+  </si>
+  <si>
+    <t>http://www.wikipathways.org/instance/WP413_r84705</t>
+  </si>
+  <si>
+    <t>wpid</t>
+  </si>
+  <si>
+    <t>mmu-miR-34b-5p</t>
+  </si>
+  <si>
+    <t>mmu-miR-34b-5p, mmu-miR-34-5p</t>
+  </si>
+  <si>
+    <t>12571, 22330</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>version</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,13 +242,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -478,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -502,16 +610,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -522,10 +630,10 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -536,7 +644,7 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -550,7 +658,7 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -564,7 +672,7 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -572,10 +680,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -586,13 +694,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -600,24 +708,24 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -628,10 +736,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -642,23 +750,63 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>27</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D12">
-    <sortCondition descending="1" ref="D1"/>
-  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -669,19 +817,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -689,243 +836,436 @@
         <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>32</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2">
+        <v>12571</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F3">
-        <v>22330</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4">
         <v>22330</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5">
         <v>22330</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6">
         <v>140484</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7">
+        <v>12571</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7">
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8">
         <v>12053</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8">
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10">
         <v>11908</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11">
+        <v>12571</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9">
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12">
         <v>22330</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10">
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13">
         <v>11908</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" t="s">
         <v>25</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11">
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14">
         <v>22330</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>27</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12">
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15">
         <v>22330</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F12">
-    <sortCondition descending="1" ref="D1"/>
-  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>